<commit_message>
paar controle bugs + stats verdere implementatie
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\planning tool praxis\PRAxIS_Planningstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0B4CC5-EFCB-430A-9F73-8FA93235A493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478D997E-07F8-4A6E-BCBD-AEA7BE75111E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15555" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11505" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="54">
   <si>
     <t>Datum</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Gui</t>
+  </si>
+  <si>
+    <t>main + web worker verder implementeren</t>
+  </si>
+  <si>
+    <t>verdere implementatie automatisatie + extra info historiebox op screen</t>
   </si>
 </sst>
 </file>
@@ -353,6 +359,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -361,12 +373,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDD1A17-043F-436A-8C89-13D933356F9D}">
   <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,10 +705,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -720,15 +726,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -894,16 +900,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="16" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -923,7 +929,7 @@
       <c r="F11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -948,7 +954,7 @@
       <c r="G12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -973,7 +979,7 @@
       <c r="G13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -998,7 +1004,7 @@
       <c r="G14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1016,7 +1022,7 @@
       <c r="F15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1041,7 +1047,7 @@
       <c r="G16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1066,19 +1072,19 @@
       <c r="G17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="17"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1096,7 +1102,7 @@
       <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1121,7 +1127,7 @@
       <c r="G20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1146,7 +1152,7 @@
       <c r="G21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1171,7 +1177,7 @@
       <c r="G22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1189,7 +1195,7 @@
       <c r="F23" s="8">
         <v>0</v>
       </c>
-      <c r="H23" s="17"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1214,7 +1220,7 @@
       <c r="G24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1239,18 +1245,18 @@
       <c r="G25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="18"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1382,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="10"/>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1402,19 +1408,19 @@
       <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="H33" s="17"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1432,7 +1438,7 @@
       <c r="F35" s="8">
         <v>0</v>
       </c>
-      <c r="H35" s="17"/>
+      <c r="H35" s="19"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -1451,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="10"/>
-      <c r="H36" s="17"/>
+      <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1469,7 +1475,7 @@
       <c r="F37" s="8">
         <v>0</v>
       </c>
-      <c r="H37" s="17"/>
+      <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1488,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="10"/>
-      <c r="H38" s="17"/>
+      <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1506,7 +1512,7 @@
       <c r="F39" s="8">
         <v>0</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -1525,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="H40" s="17"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1550,18 +1556,18 @@
       <c r="G41" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="18"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1716,15 +1722,15 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1877,15 +1883,15 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2025,26 +2031,33 @@
       <c r="B65" s="3">
         <v>44661</v>
       </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
+      <c r="C65" s="4">
+        <v>0.3125</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0.5</v>
+      </c>
       <c r="E65" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="F65" s="8">
         <v>0</v>
       </c>
+      <c r="G65" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -2070,16 +2083,22 @@
       <c r="B68" s="6">
         <v>44663</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
+      <c r="C68" s="7">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="E68" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F68" s="9">
         <v>0</v>
       </c>
-      <c r="G68" s="10"/>
+      <c r="G68" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -2169,15 +2188,15 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2302,15 +2321,15 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -2435,15 +2454,15 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
+      <c r="A90" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="19"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -2568,15 +2587,15 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="19" t="s">
+      <c r="A98" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="19"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="19"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -2701,15 +2720,15 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="19" t="s">
+      <c r="A106" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
-      <c r="G106" s="19"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -2834,15 +2853,15 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="19" t="s">
+      <c r="A114" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B114" s="19"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="19"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -2967,15 +2986,15 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="19" t="s">
+      <c r="A122" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B122" s="19"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="19"/>
+      <c r="B122" s="17"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="17"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3100,15 +3119,15 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="19" t="s">
+      <c r="A130" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B130" s="19"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="19"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -3233,15 +3252,15 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="19" t="s">
+      <c r="A138" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B138" s="19"/>
-      <c r="C138" s="19"/>
-      <c r="D138" s="19"/>
-      <c r="E138" s="19"/>
-      <c r="F138" s="19"/>
-      <c r="G138" s="19"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3370,11 +3389,11 @@
       </c>
       <c r="E147" s="15">
         <f>SUM(E3:E9,E11:E17,E19:E25,E27:E33,E35:E41,E43:E49,E52:E57,E51,E59:E65,E145)</f>
-        <v>9.9895833333333321</v>
+        <v>10.177083333333332</v>
       </c>
       <c r="F147" s="2">
         <f>E147*24</f>
-        <v>239.74999999999997</v>
+        <v>244.24999999999997</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,7 +3402,7 @@
       </c>
       <c r="F148" s="2">
         <f>F147/F149 *100</f>
-        <v>46.826171874999993</v>
+        <v>47.705078124999993</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3397,18 +3416,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A138:G138"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A82:G82"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="A106:G106"/>
     <mergeCell ref="H10:H25"/>
     <mergeCell ref="H32:H41"/>
     <mergeCell ref="A114:G114"/>
@@ -3418,6 +3425,18 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="A106:G106"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stats: calculatie nachtshiften tussen 2 maanden
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\planning tool praxis\PRAxIS_Planningstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4BCD67-5F0C-4F57-B42E-A96015DB7D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFEB2C9-51DB-4845-B317-2CF61594828E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15555" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
   <si>
     <t>Datum</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Maandoverzicht uren in historiebox</t>
+  </si>
+  <si>
+    <t>statistieken</t>
   </si>
 </sst>
 </file>
@@ -362,6 +365,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -370,12 +379,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDD1A17-043F-436A-8C89-13D933356F9D}">
   <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,10 +711,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -729,15 +732,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -903,16 +906,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="16" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -932,7 +935,7 @@
       <c r="F11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -957,7 +960,7 @@
       <c r="G12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -982,7 +985,7 @@
       <c r="G13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1007,7 +1010,7 @@
       <c r="G14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1025,7 +1028,7 @@
       <c r="F15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1050,7 +1053,7 @@
       <c r="G16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1075,19 +1078,19 @@
       <c r="G17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="17"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1105,7 +1108,7 @@
       <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1130,7 +1133,7 @@
       <c r="G20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1155,7 +1158,7 @@
       <c r="G21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1180,7 +1183,7 @@
       <c r="G22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1198,7 +1201,7 @@
       <c r="F23" s="8">
         <v>0</v>
       </c>
-      <c r="H23" s="17"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1223,7 +1226,7 @@
       <c r="G24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1248,18 +1251,18 @@
       <c r="G25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="18"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1391,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="10"/>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1411,19 +1414,19 @@
       <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="H33" s="17"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1441,7 +1444,7 @@
       <c r="F35" s="8">
         <v>0</v>
       </c>
-      <c r="H35" s="17"/>
+      <c r="H35" s="19"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -1460,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="10"/>
-      <c r="H36" s="17"/>
+      <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1478,7 +1481,7 @@
       <c r="F37" s="8">
         <v>0</v>
       </c>
-      <c r="H37" s="17"/>
+      <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1497,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="10"/>
-      <c r="H38" s="17"/>
+      <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1515,7 +1518,7 @@
       <c r="F39" s="8">
         <v>0</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -1534,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="H40" s="17"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1559,18 +1562,18 @@
       <c r="G41" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="18"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1725,15 +1728,15 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1886,15 +1889,15 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2052,15 +2055,15 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -2187,26 +2190,33 @@
       <c r="B73" s="3">
         <v>44668</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+      <c r="C73" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D73" s="4">
+        <v>1</v>
+      </c>
       <c r="E73" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F73" s="8">
         <v>1</v>
       </c>
+      <c r="G73" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2331,15 +2341,15 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -2464,15 +2474,15 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
+      <c r="A90" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="19"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -2597,15 +2607,15 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="19" t="s">
+      <c r="A98" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="19"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="19"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -2730,15 +2740,15 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="19" t="s">
+      <c r="A106" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
-      <c r="G106" s="19"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -2863,15 +2873,15 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="19" t="s">
+      <c r="A114" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B114" s="19"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="19"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -2996,15 +3006,15 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="19" t="s">
+      <c r="A122" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B122" s="19"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="19"/>
+      <c r="B122" s="17"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="17"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3129,15 +3139,15 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="19" t="s">
+      <c r="A130" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B130" s="19"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="19"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -3262,15 +3272,15 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="19" t="s">
+      <c r="A138" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B138" s="19"/>
-      <c r="C138" s="19"/>
-      <c r="D138" s="19"/>
-      <c r="E138" s="19"/>
-      <c r="F138" s="19"/>
-      <c r="G138" s="19"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3398,12 +3408,12 @@
         <v>3</v>
       </c>
       <c r="E147" s="15">
-        <f>SUM(E3:E9,E11:E17,E19:E25,E27:E33,E35:E41,E43:E49,E52:E57,E51,E59:E65,E145)</f>
-        <v>10.177083333333332</v>
+        <f>SUM(E3:E9,E11:E17,E19:E25,E27:E33,E35:E41,E43:E49,E52:E57,E51,E59:E65,E145,E67:E73)</f>
+        <v>11.218749999999998</v>
       </c>
       <c r="F147" s="2">
         <f>E147*24</f>
-        <v>244.24999999999997</v>
+        <v>269.24999999999994</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -3412,7 +3422,7 @@
       </c>
       <c r="F148" s="2">
         <f>F147/F149 *100</f>
-        <v>47.705078124999993</v>
+        <v>52.587890624999986</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3426,18 +3436,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A138:G138"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A82:G82"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="A106:G106"/>
     <mergeCell ref="H10:H25"/>
     <mergeCell ref="H32:H41"/>
     <mergeCell ref="A114:G114"/>
@@ -3447,6 +3445,18 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="A106:G106"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wijziging sidebar volgens V3
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\planning tool praxis\PRAxIS_Planningstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFEB2C9-51DB-4845-B317-2CF61594828E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B13C48B-3CEA-4963-A445-0128CB0FE361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="56">
   <si>
     <t>Datum</t>
   </si>
@@ -365,12 +365,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -379,6 +373,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDD1A17-043F-436A-8C89-13D933356F9D}">
   <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,10 +711,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -732,15 +732,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -906,16 +906,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -935,7 +935,7 @@
       <c r="F11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="19"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -960,7 +960,7 @@
       <c r="G12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -985,7 +985,7 @@
       <c r="G13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="19"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1010,7 +1010,7 @@
       <c r="G14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="19"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1028,7 +1028,7 @@
       <c r="F15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="19"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1053,7 +1053,7 @@
       <c r="G16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="19"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1078,19 +1078,19 @@
       <c r="G17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="19"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1108,7 +1108,7 @@
       <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1133,7 +1133,7 @@
       <c r="G20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="19"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1158,7 +1158,7 @@
       <c r="G21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="19"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1183,7 +1183,7 @@
       <c r="G22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="19"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1201,7 +1201,7 @@
       <c r="F23" s="8">
         <v>0</v>
       </c>
-      <c r="H23" s="19"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1226,7 +1226,7 @@
       <c r="G24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1251,18 +1251,18 @@
       <c r="G25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1394,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="10"/>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1414,19 +1414,19 @@
       <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="H33" s="19"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1444,7 +1444,7 @@
       <c r="F35" s="8">
         <v>0</v>
       </c>
-      <c r="H35" s="19"/>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="10"/>
-      <c r="H36" s="19"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1481,7 +1481,7 @@
       <c r="F37" s="8">
         <v>0</v>
       </c>
-      <c r="H37" s="19"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="10"/>
-      <c r="H38" s="19"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1518,7 +1518,7 @@
       <c r="F39" s="8">
         <v>0</v>
       </c>
-      <c r="H39" s="19"/>
+      <c r="H39" s="17"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="H40" s="19"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1562,18 +1562,18 @@
       <c r="G41" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="20"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1728,15 +1728,15 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1889,15 +1889,15 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2055,15 +2055,15 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -2208,15 +2208,15 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2242,16 +2242,22 @@
       <c r="B76" s="6">
         <v>44670</v>
       </c>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
+      <c r="C76" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D76" s="7">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="E76" s="7">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="F76" s="9">
         <v>1</v>
       </c>
-      <c r="G76" s="10"/>
+      <c r="G76" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -2277,16 +2283,22 @@
       <c r="B78" s="6">
         <v>44672</v>
       </c>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
+      <c r="C78" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="D78" s="7">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E78" s="7">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="F78" s="9">
         <v>0</v>
       </c>
-      <c r="G78" s="10"/>
+      <c r="G78" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -2341,15 +2353,15 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -2474,15 +2486,15 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -2607,15 +2619,15 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -2740,15 +2752,15 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+      <c r="A106" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B106" s="17"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="17"/>
-      <c r="G106" s="17"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="19"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -2873,15 +2885,15 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="17" t="s">
+      <c r="A114" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="17"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="19"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -3006,15 +3018,15 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
+      <c r="A122" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="17"/>
-      <c r="E122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="G122" s="17"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="19"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3139,15 +3151,15 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
+      <c r="A130" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B130" s="17"/>
-      <c r="C130" s="17"/>
-      <c r="D130" s="17"/>
-      <c r="E130" s="17"/>
-      <c r="F130" s="17"/>
-      <c r="G130" s="17"/>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="19"/>
+      <c r="G130" s="19"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -3272,15 +3284,15 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="17" t="s">
+      <c r="A138" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B138" s="17"/>
-      <c r="C138" s="17"/>
-      <c r="D138" s="17"/>
-      <c r="E138" s="17"/>
-      <c r="F138" s="17"/>
-      <c r="G138" s="17"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="19"/>
+      <c r="D138" s="19"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+      <c r="G138" s="19"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3436,6 +3448,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="A106:G106"/>
     <mergeCell ref="H10:H25"/>
     <mergeCell ref="H32:H41"/>
     <mergeCell ref="A114:G114"/>
@@ -3445,18 +3469,6 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A138:G138"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A82:G82"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="A106:G106"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Vorige commit: Shifttype ID geimplementeerd
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\planning tool praxis\PRAxIS_Planningstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA789C54-B57A-420E-86E0-64F56AEF9B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A905CF6-B653-44AA-85DA-6E4C0F04619F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>weekstructuren</t>
+  </si>
+  <si>
+    <t>wijziging shift in db</t>
+  </si>
+  <si>
+    <t>wijzinging weekstructuur</t>
   </si>
 </sst>
 </file>
@@ -377,12 +383,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -391,6 +391,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -709,7 +715,7 @@
   <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,10 +729,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -744,15 +750,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -918,16 +924,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -947,7 +953,7 @@
       <c r="F11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="19"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -972,7 +978,7 @@
       <c r="G12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -997,7 +1003,7 @@
       <c r="G13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="19"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1022,7 +1028,7 @@
       <c r="G14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="19"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1040,7 +1046,7 @@
       <c r="F15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="19"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1065,7 +1071,7 @@
       <c r="G16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="19"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1090,19 +1096,19 @@
       <c r="G17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="19"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1120,7 +1126,7 @@
       <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1145,7 +1151,7 @@
       <c r="G20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="19"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1170,7 +1176,7 @@
       <c r="G21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="19"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1195,7 +1201,7 @@
       <c r="G22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="19"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1213,7 +1219,7 @@
       <c r="F23" s="8">
         <v>0</v>
       </c>
-      <c r="H23" s="19"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1238,7 +1244,7 @@
       <c r="G24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1263,18 +1269,18 @@
       <c r="G25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1406,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="10"/>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1426,19 +1432,19 @@
       <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="H33" s="19"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1456,7 +1462,7 @@
       <c r="F35" s="8">
         <v>0</v>
       </c>
-      <c r="H35" s="19"/>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -1475,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="10"/>
-      <c r="H36" s="19"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1493,7 +1499,7 @@
       <c r="F37" s="8">
         <v>0</v>
       </c>
-      <c r="H37" s="19"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1512,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="10"/>
-      <c r="H38" s="19"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1530,7 +1536,7 @@
       <c r="F39" s="8">
         <v>0</v>
       </c>
-      <c r="H39" s="19"/>
+      <c r="H39" s="17"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -1549,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="H40" s="19"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1574,18 +1580,18 @@
       <c r="G41" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="20"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1740,15 +1746,15 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1901,15 +1907,15 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2067,15 +2073,15 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -2220,15 +2226,15 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2365,15 +2371,15 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -2385,7 +2391,7 @@
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4">
-        <f t="shared" ref="E83:E89" si="10">ABS(D83-C83)</f>
+        <f t="shared" ref="E83:E86" si="10">ABS(D83-C83)</f>
         <v>0</v>
       </c>
       <c r="F83" s="8">
@@ -2528,15 +2534,15 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -2562,16 +2568,22 @@
       <c r="B92" s="6">
         <v>44684</v>
       </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
+      <c r="C92" s="7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D92" s="7">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E92" s="7">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F92" s="9">
         <v>0</v>
       </c>
-      <c r="G92" s="10"/>
+      <c r="G92" s="10" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
@@ -2597,16 +2609,21 @@
       <c r="B94" s="6">
         <v>44686</v>
       </c>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
+      <c r="C94" s="7">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D94" s="7">
+        <v>0.1875</v>
+      </c>
       <c r="E94" s="7">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="F94" s="9">
         <v>0</v>
       </c>
-      <c r="G94" s="10"/>
+      <c r="G94" s="10" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -2661,15 +2678,15 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -2794,15 +2811,15 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+      <c r="A106" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B106" s="17"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="17"/>
-      <c r="G106" s="17"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="19"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -2927,15 +2944,15 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="17" t="s">
+      <c r="A114" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="17"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="19"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -3060,15 +3077,15 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
+      <c r="A122" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="17"/>
-      <c r="E122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="G122" s="17"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="19"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3193,15 +3210,15 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
+      <c r="A130" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B130" s="17"/>
-      <c r="C130" s="17"/>
-      <c r="D130" s="17"/>
-      <c r="E130" s="17"/>
-      <c r="F130" s="17"/>
-      <c r="G130" s="17"/>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="19"/>
+      <c r="G130" s="19"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -3326,15 +3343,15 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="17" t="s">
+      <c r="A138" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B138" s="17"/>
-      <c r="C138" s="17"/>
-      <c r="D138" s="17"/>
-      <c r="E138" s="17"/>
-      <c r="F138" s="17"/>
-      <c r="G138" s="17"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="19"/>
+      <c r="D138" s="19"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+      <c r="G138" s="19"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3490,6 +3507,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="A106:G106"/>
     <mergeCell ref="H10:H25"/>
     <mergeCell ref="H32:H41"/>
     <mergeCell ref="A114:G114"/>
@@ -3499,18 +3528,6 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A138:G138"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A82:G82"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="A106:G106"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
automatische flow uurtoekenning & weekend
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\planning tool praxis\PRAxIS_Planningstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A905CF6-B653-44AA-85DA-6E4C0F04619F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9764CD60-E754-4AB2-AC8B-05C924E66060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{306C4310-2B63-47D3-AF00-80A555A60C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
   <si>
     <t>Datum</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>wijzinging weekstructuur</t>
+  </si>
+  <si>
+    <t>wijziging automatisatieflow</t>
+  </si>
+  <si>
+    <t>wijziging automatisatieflow(uren toekenning &amp; weekend)</t>
   </si>
 </sst>
 </file>
@@ -714,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDD1A17-043F-436A-8C89-13D933356F9D}">
   <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2632,14 +2638,20 @@
       <c r="B95" s="3">
         <v>44687</v>
       </c>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
+      <c r="C95" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D95" s="4">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="E95" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="F95" s="8">
         <v>1</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2649,16 +2661,21 @@
       <c r="B96" s="6">
         <v>44688</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+      <c r="C96" s="7">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D96" s="7">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="E96" s="7">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
       <c r="F96" s="9">
         <v>1</v>
       </c>
-      <c r="G96" s="10"/>
+      <c r="G96" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">

</xml_diff>